<commit_message>
Add scripts for joining data
</commit_message>
<xml_diff>
--- a/Описание полей 3 датасетов.xlsx
+++ b/Описание полей 3 датасетов.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirill\Documents\repos\big-data-midterm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866938CF-55DE-4EF7-8D48-B0681E4C6C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41B7091-AC36-4E28-8B0F-BD779AFDF9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E904E9A8-56F9-4E7D-9D85-76ADD9A8991A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t xml:space="preserve"> 'Baggage',</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>AgentInfo',</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'PassengerDocument'</t>
   </si>
   <si>
     <t xml:space="preserve"> 'DepartureTime',</t>
@@ -518,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA895C5-33CD-4CD5-B420-EA27782FD9BA}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +534,7 @@
       </c>
       <c r="G1" s="3"/>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -549,7 +546,7 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -562,7 +559,7 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -613,8 +610,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -645,131 +644,122 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="5"/>
+      <c r="A16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A17" s="5"/>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5"/>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="C19" t="s">
-        <v>25</v>
+      <c r="B19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" t="s">
-        <v>18</v>
+      <c r="A20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>